<commit_message>
#12313 Uid changed and remove total for %,marks,rank
</commit_message>
<xml_diff>
--- a/OutputReports/DHIS2 Reports/HTML Reports/Maharashtra/RCH Reports/#12313 ANC 4 check-up Report/12. ANC 4 check-ups.xlsx
+++ b/OutputReports/DHIS2 Reports/HTML Reports/Maharashtra/RCH Reports/#12313 ANC 4 check-up Report/12. ANC 4 check-ups.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23895" windowHeight="10350"/>
+    <workbookView windowWidth="23895" windowHeight="10335"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,12 +14,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51">
   <si>
     <t>State Family Welfare Bureau,Pune</t>
   </si>
   <si>
-    <t xml:space="preserve">   Districtwise Performance of ANC TT2+ANC TT Booster (Total Marks-10)</t>
+    <t xml:space="preserve">   Districtwise Performance of ANC 4 check-up (Total Marks-10)</t>
   </si>
   <si>
     <t xml:space="preserve">Sr No </t>
@@ -70,19 +70,19 @@
     <t xml:space="preserve">Annual </t>
   </si>
   <si>
-    <t>yD38I0iiRiz.HllvX50cXC0</t>
+    <t>XsN6kzcCUuK.HllvX50cXC0</t>
   </si>
   <si>
     <t>(C/12)*no. Of months</t>
   </si>
   <si>
-    <t>m5ZMShcazP2.ZnztZgggxd6 + zYnye4A85aP.ZnztZgggxd6</t>
+    <t>g17APAT44NM.ZnztZgggxd6</t>
   </si>
   <si>
     <t>E column's cumulative data (upto that month in financial year)</t>
   </si>
   <si>
-    <t>m5ZMShcazP2.DLr4VIEGNIo + zYnye4A85aP.DLr4VIEGNIo</t>
+    <t>g17APAT44NM.DLr4VIEGNIo</t>
   </si>
   <si>
     <t>H column's cumulative data (upto that month in financial year)</t>
@@ -116,64 +116,58 @@
     <t>1. Use following groups for District Total fields:</t>
   </si>
   <si>
-    <t>District:-</t>
-  </si>
-  <si>
-    <t>Rural Group</t>
-  </si>
-  <si>
     <t>DH - Rural</t>
   </si>
   <si>
     <t>GH Group</t>
   </si>
   <si>
-    <t>Corporation:-</t>
+    <t>MCL Group</t>
+  </si>
+  <si>
+    <t>RH Group</t>
+  </si>
+  <si>
+    <t>SDH 100 Group</t>
+  </si>
+  <si>
+    <t>SDH 50 Group</t>
+  </si>
+  <si>
+    <t>WH Group</t>
+  </si>
+  <si>
+    <t>PHC - Rural</t>
+  </si>
+  <si>
+    <t>SC Group</t>
+  </si>
+  <si>
+    <t>Cantonment group</t>
+  </si>
+  <si>
+    <t>Rural Facility group</t>
+  </si>
+  <si>
+    <t>2. Use following groups for Corporation total fields:</t>
+  </si>
+  <si>
+    <t>UPHC Group</t>
+  </si>
+  <si>
+    <t>UCHC Group</t>
+  </si>
+  <si>
+    <t>USDH Group</t>
+  </si>
+  <si>
+    <t>UDH Group</t>
   </si>
   <si>
     <t>Corporation Group</t>
   </si>
   <si>
-    <t>MCL Group</t>
-  </si>
-  <si>
-    <t>RH Group</t>
-  </si>
-  <si>
-    <t>SDH 100 Group</t>
-  </si>
-  <si>
-    <t>SDH 50 Group</t>
-  </si>
-  <si>
-    <t>WH Group</t>
-  </si>
-  <si>
-    <t>PHC - Rural</t>
-  </si>
-  <si>
-    <t>SC Group</t>
-  </si>
-  <si>
-    <t>Cantonment group</t>
-  </si>
-  <si>
-    <t>Rural Facility group</t>
-  </si>
-  <si>
-    <t>2. Use following groups for Corporation total fields:</t>
-  </si>
-  <si>
-    <t>UPHC Group</t>
-  </si>
-  <si>
-    <t>UCHC Group</t>
-  </si>
-  <si>
-    <t>USDH Group</t>
-  </si>
-  <si>
-    <t>UDH Group</t>
+    <t>PMP facility</t>
   </si>
 </sst>
 </file>
@@ -181,10 +175,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="27">
     <font>
@@ -241,6 +235,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -248,14 +249,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -270,7 +272,61 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -284,101 +340,39 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -405,103 +399,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -513,79 +579,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -675,6 +669,39 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -707,30 +734,6 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -743,8 +746,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -763,21 +766,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -795,130 +789,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="14" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="22" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="22" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1291,10 +1285,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:P25"/>
+  <dimension ref="A1:P26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -1428,7 +1422,7 @@
       <c r="O4" s="8"/>
       <c r="P4" s="8"/>
     </row>
-    <row r="5" ht="60" spans="1:16">
+    <row r="5" ht="45" spans="1:16">
       <c r="A5" s="9"/>
       <c r="B5" s="9"/>
       <c r="C5" s="10" t="s">
@@ -1479,101 +1473,94 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="4:7">
-      <c r="D8" t="s">
+    <row r="8" spans="7:7">
+      <c r="G8" s="15" t="s">
         <v>33</v>
-      </c>
-      <c r="E8" t="s">
-        <v>34</v>
-      </c>
-      <c r="G8" s="15" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="9" spans="7:7">
       <c r="G9" s="15" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="10" spans="4:7">
-      <c r="D10" t="s">
-        <v>37</v>
-      </c>
-      <c r="E10" t="s">
-        <v>38</v>
-      </c>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="7:7">
       <c r="G10" s="15" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="7:7">
       <c r="G11" s="15" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="7:7">
       <c r="G12" s="15" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="7:7">
       <c r="G13" s="15" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="7:7">
       <c r="G14" s="15" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15" spans="7:7">
       <c r="G15" s="15" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="16" spans="7:7">
       <c r="G16" s="15" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="17" spans="7:7">
       <c r="G17" s="15" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="18" spans="7:7">
       <c r="G18" s="15" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="20" ht="45" spans="7:7">
       <c r="G20" s="14" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="21" spans="7:7">
       <c r="G21" s="15" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="22" spans="7:7">
       <c r="G22" s="15" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="23" spans="7:7">
       <c r="G23" s="15" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="24" spans="7:7">
       <c r="G24" s="15" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="25" spans="7:7">
       <c r="G25" s="15" t="s">
-        <v>38</v>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="26" spans="7:7">
+      <c r="G26" s="15" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>